<commit_message>
modification to theme and timeline
</commit_message>
<xml_diff>
--- a/timeline.xlsx
+++ b/timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suyif\Desktop\Colum 1#\BISTP8105 - Data Science I\p8105_final_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chenxin\Desktop\aDS\p8105_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAF290C-434A-4266-B549-D8872B59D6D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1F2E8B-F59E-45FD-8169-EF9A8237F95B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9090" yWindow="180" windowWidth="9420" windowHeight="9450" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mlb11" sheetId="1" r:id="rId1"/>
@@ -28,50 +28,98 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+  <si>
+    <t>Objectives</t>
+  </si>
+  <si>
+    <t>set goals and have a proposal</t>
+  </si>
+  <si>
+    <t>hand in the proposal</t>
+  </si>
+  <si>
+    <t>tidy the data, preliminary work</t>
+  </si>
+  <si>
+    <t>meet with TA, make correction</t>
+  </si>
+  <si>
+    <t>started to write the final report</t>
+  </si>
+  <si>
+    <t>polise final report, screencast, webpages</t>
+  </si>
+  <si>
+    <t>do peer assessment</t>
+  </si>
+  <si>
+    <t>in-class discussion of projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tidy data, basic frames of the website</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Objectives</t>
-  </si>
-  <si>
-    <t>set goals and have a proposal</t>
-  </si>
-  <si>
-    <t>hand in the proposal</t>
-  </si>
-  <si>
-    <t>tidy the data, preliminary work</t>
-  </si>
-  <si>
-    <t>meet with TA, make correction</t>
-  </si>
-  <si>
-    <t>have tidy data, basic frames of the website</t>
-  </si>
-  <si>
-    <t>started to write the final report</t>
-  </si>
-  <si>
-    <t>have group meeting, complete report and the website</t>
-  </si>
-  <si>
-    <t>polise final report, screencast, webpages</t>
-  </si>
-  <si>
-    <t>do peer assessment</t>
-  </si>
-  <si>
-    <t>in-class discussion of projects</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Objective</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11/29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>12/10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>meeting, complete report and website</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="mm/dd/yy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="m/d;@"/>
+    <numFmt numFmtId="177" formatCode="mm/dd"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -109,14 +157,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -397,107 +448,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="H1:I11"/>
+  <dimension ref="H1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15.5"/>
   <cols>
+    <col min="8" max="8" width="11.07421875" style="3"/>
     <col min="9" max="9" width="46.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.07421875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:9">
-      <c r="H1" s="1" t="s">
+    <row r="1" spans="8:12">
+      <c r="H1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="8:12">
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="8:9">
-      <c r="H2" s="2">
-        <v>44141</v>
-      </c>
-      <c r="I2" s="1" t="s">
+    <row r="3" spans="8:12">
+      <c r="H3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="3" spans="8:9">
-      <c r="H3" s="2">
-        <v>44142</v>
-      </c>
-      <c r="I3" s="1" t="s">
+    <row r="4" spans="8:12">
+      <c r="H4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="J4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="4" spans="8:9">
-      <c r="H4" s="2">
-        <v>44145</v>
-      </c>
-      <c r="I4" s="1" t="s">
+    <row r="5" spans="8:12">
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="8:9">
-      <c r="H5" s="2">
-        <v>44147</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="8:9">
-      <c r="H6" s="2">
-        <v>44155</v>
+    <row r="6" spans="8:12">
+      <c r="H6" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="8:9">
-      <c r="H7" s="2">
-        <v>44160</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="8:9">
-      <c r="H8" s="2">
-        <v>44164</v>
-      </c>
-      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="8:9">
-      <c r="H9" s="2">
-        <v>44169</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="8:9">
-      <c r="H10" s="2">
-        <v>44173</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="8:9">
-      <c r="H11" s="2">
-        <v>44175</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>